<commit_message>
Correction in get_excel(df, nombre)
</commit_message>
<xml_diff>
--- a/Programacion Data Science/Practica4/population.xlsx
+++ b/Programacion Data Science/Practica4/population.xlsx
@@ -104,14 +104,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF008000"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>

</xml_diff>

<commit_message>
Modification in get_excel function
</commit_message>
<xml_diff>
--- a/Programacion Data Science/Practica4/population.xlsx
+++ b/Programacion Data Science/Practica4/population.xlsx
@@ -86,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +105,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -160,6 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,16 +596,16 @@
       <c r="K3" s="4">
         <v>973</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="5">
         <v>1022</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="5">
         <v>1052</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="5">
         <v>2478</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="5">
         <v>2308</v>
       </c>
     </row>
@@ -626,25 +634,25 @@
       <c r="H4" s="4">
         <v>947</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <v>1402</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="5">
         <v>3700</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="5">
         <v>4054</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="5">
         <v>4164</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="5">
         <v>4250</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="5">
         <v>5267</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="5">
         <v>5561</v>
       </c>
     </row>

</xml_diff>